<commit_message>
adding new feature to handle the blue split leather export
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/JF.xlsx
+++ b/invoice_gen/TEMPLATE/JF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\automate invoice\invoice_gen\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\inv_pkl_contract_creation - Copy\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798D18C3-E880-4B9D-B524-8AD677924DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3D9948-3BBB-4DDF-A3AE-DF6A8B5C818A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
   <si>
     <t>SALES CONTRACT</t>
   </si>
@@ -74,34 +74,6 @@
   </si>
   <si>
     <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 55, 56</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t>，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>AREA B2, DONG XOAI III INDUSTRIAL ZONE, TIEN HUNG COMMUNE,</t>
-    </r>
-  </si>
-  <si>
-    <t>DONG XOAI CITY, BINH PHUOC PROVINCE, VIETNAM.</t>
   </si>
   <si>
     <t>Contact Person : Contact Person : Mr. Thuy   Tel: 0379367084</t>
@@ -234,12 +206,6 @@
     <t>CONSIGNEE :</t>
   </si>
   <si>
-    <t xml:space="preserve">LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，AREA B2, DONG XOAI III INDUSTRIAL ZONE, </t>
-  </si>
-  <si>
-    <t>TIEN HUNG COMMUNE, DONG XOAI CITY, BINH PHUOC PROVINCE, VIETNAM.</t>
-  </si>
-  <si>
     <t>Contact Person : Mr. Thuy   TEl: 0379367084</t>
   </si>
   <si>
@@ -250,9 +216,6 @@
   </si>
   <si>
     <t xml:space="preserve">SHIP: </t>
-  </si>
-  <si>
-    <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO BINH PHUOC PROVINCE, VIETNAM.</t>
   </si>
   <si>
     <t>Country of Original Cambodia</t>
@@ -333,9 +296,6 @@
     <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
   </si>
   <si>
-    <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，AREA B2, DONG XOAI III INDUSTRIAL ZONE,</t>
-  </si>
-  <si>
     <t>EMAlL:jyangbin4720@dingtalk.com jialy@kukahome.com</t>
   </si>
   <si>
@@ -391,6 +351,15 @@
   <si>
     <t>BAVET, SVAY RIENG</t>
   </si>
+  <si>
+    <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
+  </si>
+  <si>
+    <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
+  </si>
+  <si>
+    <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
+  </si>
 </sst>
 </file>
 
@@ -403,7 +372,7 @@
     <numFmt numFmtId="166" formatCode="###0;###0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,10 +536,6 @@
     </font>
     <font>
       <sz val="15"/>
-      <name val="SimSun"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -636,6 +601,19 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -696,13 +674,13 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -836,8 +814,11 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -845,9 +826,6 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -857,14 +835,14 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -919,9 +897,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -934,22 +912,34 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -984,12 +974,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1679,8 +1663,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="15"/>
@@ -1695,13 +1679,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45.95" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
     </row>
     <row r="2" spans="1:5" s="35" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="38"/>
@@ -1717,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="35" customFormat="1" ht="30" customHeight="1">
@@ -1728,7 +1712,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="57" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1">
@@ -1770,48 +1754,57 @@
     </row>
     <row r="10" spans="1:5" s="36" customFormat="1" ht="45" customHeight="1">
       <c r="A10" s="41"/>
-      <c r="B10" s="90" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
+      <c r="B10" s="94" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="94" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="94" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="94" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1">
       <c r="A11" s="41"/>
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="94" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="36" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="41"/>
+    </row>
+    <row r="13" spans="1:5" s="36" customFormat="1" ht="60.95" customHeight="1">
+      <c r="A13" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-    </row>
-    <row r="12" spans="1:5" s="36" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="93" t="s">
+      <c r="B13" s="97"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+    </row>
+    <row r="14" spans="1:5" s="36" customFormat="1" ht="54.95" customHeight="1">
+      <c r="A14" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="93"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="41"/>
-    </row>
-    <row r="13" spans="1:5" s="36" customFormat="1" ht="60.95" customHeight="1">
-      <c r="A13" s="90" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-    </row>
-    <row r="14" spans="1:5" s="36" customFormat="1" ht="54.95" customHeight="1">
-      <c r="A14" s="91" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="91"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
     </row>
     <row r="15" spans="1:5" ht="15.75">
       <c r="A15" s="44"/>
@@ -1821,18 +1814,18 @@
       <c r="E15" s="44"/>
     </row>
     <row r="16" spans="1:5" ht="27.95" customHeight="1">
-      <c r="A16" s="94"/>
-      <c r="B16" s="94"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="98"/>
       <c r="C16" s="59"/>
       <c r="D16" s="59"/>
       <c r="E16" s="59"/>
     </row>
     <row r="17" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
       <c r="A17" s="45" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C17" s="41"/>
       <c r="D17" s="41"/>
@@ -1840,7 +1833,7 @@
     </row>
     <row r="18" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
       <c r="A18" s="41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
@@ -1849,7 +1842,7 @@
     </row>
     <row r="19" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
       <c r="A19" s="41" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
@@ -1858,7 +1851,7 @@
     </row>
     <row r="20" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
       <c r="A20" s="41" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="41"/>
       <c r="C20" s="41" t="s">
@@ -1869,44 +1862,44 @@
     </row>
     <row r="21" spans="1:6" s="36" customFormat="1" ht="45.95" customHeight="1">
       <c r="A21" s="41" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="41"/>
-      <c r="C21" s="91" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
+      <c r="C21" s="95" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
     </row>
     <row r="22" spans="1:6" s="36" customFormat="1" ht="41.1" customHeight="1">
       <c r="A22" s="41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="41"/>
-      <c r="C22" s="91" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
+      <c r="C22" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
     </row>
     <row r="23" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
       <c r="A23" s="41" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="41"/>
-      <c r="C23" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="92"/>
-      <c r="E23" s="92"/>
+      <c r="C23" s="96" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
     </row>
     <row r="24" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
       <c r="A24" s="41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
@@ -1921,10 +1914,10 @@
     </row>
     <row r="26" spans="1:6" s="37" customFormat="1" ht="29.1" customHeight="1">
       <c r="A26" s="37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D26" s="47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="37" customFormat="1" ht="57" customHeight="1">
@@ -1939,13 +1932,12 @@
       <c r="E27" s="73"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C23:E23"/>
-    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A16:B16"/>
@@ -1965,7 +1957,7 @@
   <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1976,7 +1968,7 @@
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="25.140625" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
@@ -1984,70 +1976,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="99" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+    </row>
+    <row r="2" spans="1:7" ht="24" customHeight="1">
+      <c r="A2" s="100" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A3" s="101" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A4" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-    </row>
-    <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="96" t="s">
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+    </row>
+    <row r="5" spans="1:7" ht="25.5" customHeight="1">
+      <c r="A5" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-    </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="97" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-    </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="96" t="s">
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+    </row>
+    <row r="6" spans="1:7" ht="83.25" customHeight="1">
+      <c r="A6" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-    </row>
-    <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="98" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-    </row>
-    <row r="6" spans="1:7" ht="83.25" customHeight="1">
-      <c r="A6" s="100" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="100"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="4"/>
@@ -2056,57 +2048,57 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G7" s="58" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G8" s="86" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G9" s="88" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="22.5" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="106" t="s">
-        <v>68</v>
+        <v>39</v>
+      </c>
+      <c r="G10" s="89" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.25" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -2123,7 +2115,7 @@
     </row>
     <row r="13" spans="1:7" ht="25.5" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>10</v>
@@ -2134,8 +2126,8 @@
     </row>
     <row r="14" spans="1:7" ht="25.5" customHeight="1">
       <c r="A14" s="4"/>
-      <c r="B14" s="13" t="s">
-        <v>43</v>
+      <c r="B14" s="63" t="s">
+        <v>64</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -2144,8 +2136,8 @@
     </row>
     <row r="15" spans="1:7" ht="25.5" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="16" t="s">
-        <v>44</v>
+      <c r="B15" s="64" t="s">
+        <v>65</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2155,7 +2147,7 @@
     <row r="16" spans="1:7" ht="25.5" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -2165,7 +2157,7 @@
     <row r="17" spans="1:15" ht="25.5" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -2175,7 +2167,7 @@
     <row r="18" spans="1:15" ht="25.5" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2184,10 +2176,10 @@
     </row>
     <row r="19" spans="1:15" ht="27.75" customHeight="1">
       <c r="A19" s="19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -2213,11 +2205,11 @@
       <c r="O22" s="51"/>
     </row>
     <row r="23" spans="1:15" ht="42" customHeight="1">
-      <c r="A23" s="101" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="101"/>
-      <c r="C23" s="101"/>
+      <c r="A23" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="105"/>
+      <c r="C23" s="105"/>
       <c r="D23" s="23"/>
       <c r="E23" s="4"/>
       <c r="F23" s="33"/>
@@ -2229,12 +2221,12 @@
     </row>
     <row r="24" spans="1:15" ht="61.5" customHeight="1">
       <c r="A24" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="102" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="102"/>
+        <v>46</v>
+      </c>
+      <c r="B24" s="106" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="106"/>
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
       <c r="F24" s="4"/>
@@ -2245,11 +2237,11 @@
       <c r="O24" s="51"/>
     </row>
     <row r="25" spans="1:15" ht="42" customHeight="1">
-      <c r="A25" s="103" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="103"/>
-      <c r="C25" s="103"/>
+      <c r="A25" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="107"/>
+      <c r="C25" s="107"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
@@ -2260,30 +2252,30 @@
       <c r="O25" s="51"/>
     </row>
     <row r="26" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A26" s="99" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="99"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="99"/>
-      <c r="F26" s="99"/>
-      <c r="G26" s="99"/>
+      <c r="A26" s="103" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="103"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="103"/>
       <c r="L26" s="49"/>
       <c r="M26" s="50"/>
       <c r="N26" s="51"/>
       <c r="O26" s="51"/>
     </row>
     <row r="27" spans="1:15" s="1" customFormat="1" ht="27" customHeight="1">
-      <c r="A27" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="99"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="99"/>
-      <c r="E27" s="99"/>
-      <c r="F27" s="99"/>
-      <c r="G27" s="99"/>
+      <c r="A27" s="103" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="103"/>
       <c r="L27" s="49"/>
       <c r="M27" s="50"/>
       <c r="N27" s="51"/>
@@ -2291,7 +2283,7 @@
     </row>
     <row r="28" spans="1:15" ht="45" customHeight="1">
       <c r="E28" s="81" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F28" s="81"/>
       <c r="G28" s="81"/>
@@ -2305,7 +2297,7 @@
       <c r="D29" s="78"/>
       <c r="E29" s="76"/>
       <c r="F29" s="79" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G29" s="80"/>
       <c r="L29" s="49"/>
@@ -2337,7 +2329,7 @@
       <c r="D32" s="78"/>
       <c r="E32" s="76"/>
       <c r="F32" s="77" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G32" s="77"/>
       <c r="L32" s="49"/>
@@ -2453,8 +2445,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -2466,7 +2458,7 @@
     <col min="5" max="6" width="15" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
     <col min="11" max="11" width="12.85546875"/>
     <col min="12" max="12" width="12.5703125"/>
@@ -2475,82 +2467,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" customHeight="1">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="99" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+    </row>
+    <row r="2" spans="1:9" ht="24" customHeight="1">
+      <c r="A2" s="100" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+    </row>
+    <row r="3" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A3" s="101" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+    </row>
+    <row r="4" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A4" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-    </row>
-    <row r="2" spans="1:9" ht="24" customHeight="1">
-      <c r="A2" s="96" t="s">
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+    </row>
+    <row r="5" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A5" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-    </row>
-    <row r="3" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A3" s="97" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-    </row>
-    <row r="4" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A4" s="96" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-    </row>
-    <row r="5" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A5" s="98" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="105"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
     </row>
     <row r="6" spans="1:9" ht="54" customHeight="1">
-      <c r="A6" s="100" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="100"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
+      <c r="A6" s="104" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1">
       <c r="A7" s="4"/>
@@ -2561,60 +2553,60 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I7" s="87" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I8" s="85" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="60" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I9" s="88" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="22.5" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="60" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="107" t="s">
-        <v>69</v>
+        <v>39</v>
+      </c>
+      <c r="I10" s="90" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="20.25" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="60" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -2634,7 +2626,7 @@
     </row>
     <row r="13" spans="1:9" ht="25.5" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="62" t="s">
         <v>10</v>
@@ -2646,8 +2638,8 @@
     </row>
     <row r="14" spans="1:9" ht="25.5" customHeight="1">
       <c r="A14" s="4"/>
-      <c r="B14" s="63" t="s">
-        <v>61</v>
+      <c r="B14" s="91" t="s">
+        <v>64</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -2658,8 +2650,8 @@
     </row>
     <row r="15" spans="1:9" ht="21" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="64" t="s">
-        <v>44</v>
+      <c r="B15" s="92" t="s">
+        <v>65</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2671,7 +2663,7 @@
     <row r="16" spans="1:9" ht="21" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="64" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -2683,7 +2675,7 @@
     <row r="17" spans="1:8" ht="21" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="64" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -2695,7 +2687,7 @@
     <row r="18" spans="1:8" ht="21" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="64" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2706,10 +2698,10 @@
     </row>
     <row r="19" spans="1:8" ht="27.75" customHeight="1">
       <c r="A19" s="19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B19" s="60" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="27.75" customHeight="1">
@@ -2722,7 +2714,7 @@
     </row>
     <row r="22" spans="1:8" ht="27.75" customHeight="1">
       <c r="A22" s="13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -2734,25 +2726,25 @@
     </row>
     <row r="23" spans="1:8" ht="65.25" customHeight="1">
       <c r="A23" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="104" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="104"/>
-      <c r="D23" s="104"/>
+        <v>46</v>
+      </c>
+      <c r="B23" s="108" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="51.75" customHeight="1">
-      <c r="A24" s="104" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="104"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
+      <c r="A24" s="108" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="108"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="108"/>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
@@ -2760,7 +2752,7 @@
     </row>
     <row r="25" spans="1:8" ht="27.75" customHeight="1">
       <c r="A25" s="70" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B25" s="70"/>
       <c r="C25" s="70"/>
@@ -2772,7 +2764,7 @@
     </row>
     <row r="26" spans="1:8" ht="27.75" customHeight="1">
       <c r="A26" s="70" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B26" s="70"/>
       <c r="C26" s="70"/>
@@ -2788,10 +2780,9 @@
       <c r="C27" s="82"/>
       <c r="D27" s="82"/>
       <c r="E27" s="84"/>
-      <c r="F27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="H27" s="84"/>
     </row>
     <row r="28" spans="1:8" ht="27.75" customHeight="1"/>

</xml_diff>